<commit_message>
fnished everything but schewmatic
</commit_message>
<xml_diff>
--- a/Lab 2/02_Digital_Data_Collection_Tables.xlsx
+++ b/Lab 2/02_Digital_Data_Collection_Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\LaTeX\MEC E 301\Lab 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0A7EA7-16B3-40A2-B72E-76BA397FA4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F969B7BB-60B0-4E82-9AB1-9810B1B5B151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Student Info and Rubric" sheetId="4" r:id="rId1"/>
@@ -541,6 +541,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -559,26 +573,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -973,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4B5DFEB-27AC-C14C-9885-2E931D118C39}">
   <dimension ref="A1:V144"/>
   <sheetViews>
-    <sheetView topLeftCell="A126" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N101" sqref="N101"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1061,7 +1061,7 @@
       <c r="S4"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="40">
+      <c r="A5" s="46">
         <v>0.10199999999999999</v>
       </c>
       <c r="B5">
@@ -1087,7 +1087,7 @@
       <c r="S5"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
+      <c r="A6" s="47"/>
       <c r="B6">
         <v>9.2999999999999999E-2</v>
       </c>
@@ -1111,7 +1111,7 @@
       <c r="S6" s="16"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
+      <c r="A7" s="47"/>
       <c r="B7">
         <v>9.2999999999999999E-2</v>
       </c>
@@ -1135,7 +1135,7 @@
       <c r="S7" s="16"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
+      <c r="A8" s="47"/>
       <c r="B8">
         <v>9.2999999999999999E-2</v>
       </c>
@@ -1159,7 +1159,7 @@
       <c r="S8" s="16"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
+      <c r="A9" s="47"/>
       <c r="B9">
         <v>9.2999999999999999E-2</v>
       </c>
@@ -1183,7 +1183,7 @@
       <c r="S9" s="16"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
+      <c r="A10" s="47"/>
       <c r="B10">
         <v>9.2999999999999999E-2</v>
       </c>
@@ -1207,7 +1207,7 @@
       <c r="S10" s="16"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
+      <c r="A11" s="47"/>
       <c r="B11">
         <v>9.2999999999999999E-2</v>
       </c>
@@ -1231,7 +1231,7 @@
       <c r="S11" s="16"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
+      <c r="A12" s="47"/>
       <c r="B12">
         <v>9.2999999999999999E-2</v>
       </c>
@@ -1255,7 +1255,7 @@
       <c r="S12" s="16"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
+      <c r="A13" s="47"/>
       <c r="B13">
         <v>9.8000000000000004E-2</v>
       </c>
@@ -1279,7 +1279,7 @@
       <c r="S13" s="16"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
+      <c r="A14" s="48"/>
       <c r="B14" s="10">
         <v>9.2999999999999999E-2</v>
       </c>
@@ -1303,7 +1303,7 @@
       <c r="S14" s="16"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="43">
+      <c r="A15" s="49">
         <v>1.024</v>
       </c>
       <c r="B15">
@@ -1318,7 +1318,7 @@
       <c r="E15" s="2">
         <v>1.016</v>
       </c>
-      <c r="F15" s="46"/>
+      <c r="F15" s="42"/>
       <c r="O15" s="16"/>
       <c r="P15" s="17"/>
       <c r="Q15" s="16"/>
@@ -1326,7 +1326,7 @@
       <c r="S15" s="16"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
+      <c r="A16" s="50"/>
       <c r="B16">
         <v>1.0249999999999999</v>
       </c>
@@ -1339,7 +1339,7 @@
       <c r="E16" s="2">
         <v>1.016</v>
       </c>
-      <c r="F16" s="47"/>
+      <c r="F16" s="43"/>
       <c r="O16" s="16"/>
       <c r="P16" s="17"/>
       <c r="Q16" s="16"/>
@@ -1347,7 +1347,7 @@
       <c r="S16" s="16"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
+      <c r="A17" s="50"/>
       <c r="B17">
         <v>1.0249999999999999</v>
       </c>
@@ -1360,7 +1360,7 @@
       <c r="E17" s="2">
         <v>1.016</v>
       </c>
-      <c r="F17" s="47"/>
+      <c r="F17" s="43"/>
       <c r="O17" s="16"/>
       <c r="P17" s="17"/>
       <c r="Q17" s="16"/>
@@ -1368,7 +1368,7 @@
       <c r="S17" s="16"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="50"/>
       <c r="B18">
         <v>1.0249999999999999</v>
       </c>
@@ -1381,7 +1381,7 @@
       <c r="E18" s="2">
         <v>1.016</v>
       </c>
-      <c r="F18" s="47"/>
+      <c r="F18" s="43"/>
       <c r="O18" s="16"/>
       <c r="P18" s="17"/>
       <c r="Q18" s="16"/>
@@ -1389,7 +1389,7 @@
       <c r="S18" s="16"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="50"/>
       <c r="B19">
         <v>1.0249999999999999</v>
       </c>
@@ -1402,7 +1402,7 @@
       <c r="E19" s="2">
         <v>1.016</v>
       </c>
-      <c r="F19" s="47"/>
+      <c r="F19" s="43"/>
       <c r="O19" s="16"/>
       <c r="P19" s="17"/>
       <c r="Q19" s="16"/>
@@ -1410,7 +1410,7 @@
       <c r="S19" s="16"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="50"/>
       <c r="B20">
         <v>1.0249999999999999</v>
       </c>
@@ -1423,7 +1423,7 @@
       <c r="E20" s="2">
         <v>1.016</v>
       </c>
-      <c r="F20" s="47"/>
+      <c r="F20" s="43"/>
       <c r="O20" s="16"/>
       <c r="P20" s="17"/>
       <c r="Q20" s="16"/>
@@ -1431,7 +1431,7 @@
       <c r="S20" s="16"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
+      <c r="A21" s="50"/>
       <c r="B21">
         <v>1.0249999999999999</v>
       </c>
@@ -1444,7 +1444,7 @@
       <c r="E21" s="2">
         <v>1.016</v>
       </c>
-      <c r="F21" s="47"/>
+      <c r="F21" s="43"/>
       <c r="O21" s="16"/>
       <c r="P21" s="17"/>
       <c r="Q21" s="16"/>
@@ -1452,7 +1452,7 @@
       <c r="S21" s="16"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
+      <c r="A22" s="50"/>
       <c r="B22">
         <v>1.0249999999999999</v>
       </c>
@@ -1465,7 +1465,7 @@
       <c r="E22" s="2">
         <v>1.016</v>
       </c>
-      <c r="F22" s="47"/>
+      <c r="F22" s="43"/>
       <c r="O22" s="16"/>
       <c r="P22" s="17"/>
       <c r="Q22" s="16"/>
@@ -1473,7 +1473,7 @@
       <c r="S22" s="16"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="50"/>
       <c r="B23">
         <v>1.0249999999999999</v>
       </c>
@@ -1486,7 +1486,7 @@
       <c r="E23" s="2">
         <v>1.016</v>
       </c>
-      <c r="F23" s="47"/>
+      <c r="F23" s="43"/>
       <c r="O23" s="16"/>
       <c r="P23" s="17"/>
       <c r="Q23" s="16"/>
@@ -1494,7 +1494,7 @@
       <c r="S23" s="16"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="45"/>
+      <c r="A24" s="51"/>
       <c r="B24" s="10">
         <v>1.0249999999999999</v>
       </c>
@@ -1507,7 +1507,7 @@
       <c r="E24" s="2">
         <v>1.016</v>
       </c>
-      <c r="F24" s="48"/>
+      <c r="F24" s="44"/>
       <c r="O24" s="16"/>
       <c r="P24" s="17"/>
       <c r="Q24" s="16"/>
@@ -1515,7 +1515,7 @@
       <c r="S24" s="16"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="40">
+      <c r="A25" s="46">
         <v>1.8</v>
       </c>
       <c r="B25">
@@ -1530,7 +1530,7 @@
       <c r="E25" s="11">
         <v>1.7969999999999999</v>
       </c>
-      <c r="F25" s="46"/>
+      <c r="F25" s="42"/>
       <c r="O25" s="16"/>
       <c r="P25" s="16"/>
       <c r="Q25" s="16"/>
@@ -1538,7 +1538,7 @@
       <c r="S25" s="16"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
+      <c r="A26" s="47"/>
       <c r="B26">
         <v>1.821</v>
       </c>
@@ -1551,7 +1551,7 @@
       <c r="E26" s="2">
         <v>1.7969999999999999</v>
       </c>
-      <c r="F26" s="47"/>
+      <c r="F26" s="43"/>
       <c r="O26" s="16"/>
       <c r="P26" s="16"/>
       <c r="Q26" s="16"/>
@@ -1559,7 +1559,7 @@
       <c r="S26" s="16"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="41"/>
+      <c r="A27" s="47"/>
       <c r="B27">
         <v>1.8120000000000001</v>
       </c>
@@ -1572,7 +1572,7 @@
       <c r="E27" s="2">
         <v>1.7969999999999999</v>
       </c>
-      <c r="F27" s="47"/>
+      <c r="F27" s="43"/>
       <c r="O27" s="16"/>
       <c r="P27" s="16"/>
       <c r="Q27" s="16"/>
@@ -1580,7 +1580,7 @@
       <c r="S27" s="16"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="41"/>
+      <c r="A28" s="47"/>
       <c r="B28">
         <v>1.8160000000000001</v>
       </c>
@@ -1593,7 +1593,7 @@
       <c r="E28" s="2">
         <v>1.7969999999999999</v>
       </c>
-      <c r="F28" s="47"/>
+      <c r="F28" s="43"/>
       <c r="O28" s="16"/>
       <c r="P28" s="16"/>
       <c r="Q28" s="16"/>
@@ -1601,7 +1601,7 @@
       <c r="S28" s="16"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
+      <c r="A29" s="47"/>
       <c r="B29">
         <v>1.8120000000000001</v>
       </c>
@@ -1614,7 +1614,7 @@
       <c r="E29" s="2">
         <v>1.7969999999999999</v>
       </c>
-      <c r="F29" s="47"/>
+      <c r="F29" s="43"/>
       <c r="O29" s="16"/>
       <c r="P29" s="16"/>
       <c r="Q29" s="16"/>
@@ -1622,7 +1622,7 @@
       <c r="S29" s="16"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
+      <c r="A30" s="47"/>
       <c r="B30">
         <v>1.8120000000000001</v>
       </c>
@@ -1635,7 +1635,7 @@
       <c r="E30" s="2">
         <v>1.7969999999999999</v>
       </c>
-      <c r="F30" s="47"/>
+      <c r="F30" s="43"/>
       <c r="O30" s="16"/>
       <c r="P30" s="16"/>
       <c r="Q30" s="16"/>
@@ -1643,7 +1643,7 @@
       <c r="S30" s="16"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="41"/>
+      <c r="A31" s="47"/>
       <c r="B31">
         <v>1.8160000000000001</v>
       </c>
@@ -1656,7 +1656,7 @@
       <c r="E31" s="2">
         <v>1.7969999999999999</v>
       </c>
-      <c r="F31" s="47"/>
+      <c r="F31" s="43"/>
       <c r="O31" s="16"/>
       <c r="P31" s="16"/>
       <c r="Q31" s="16"/>
@@ -1664,7 +1664,7 @@
       <c r="S31" s="16"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="41"/>
+      <c r="A32" s="47"/>
       <c r="B32">
         <v>1.8160000000000001</v>
       </c>
@@ -1677,7 +1677,7 @@
       <c r="E32" s="2">
         <v>1.7969999999999999</v>
       </c>
-      <c r="F32" s="47"/>
+      <c r="F32" s="43"/>
       <c r="O32" s="16"/>
       <c r="P32" s="16"/>
       <c r="Q32" s="16"/>
@@ -1685,7 +1685,7 @@
       <c r="S32" s="16"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="41"/>
+      <c r="A33" s="47"/>
       <c r="B33">
         <v>1.8120000000000001</v>
       </c>
@@ -1698,7 +1698,7 @@
       <c r="E33" s="2">
         <v>1.7969999999999999</v>
       </c>
-      <c r="F33" s="47"/>
+      <c r="F33" s="43"/>
       <c r="O33" s="16"/>
       <c r="P33" s="16"/>
       <c r="Q33" s="16"/>
@@ -1706,7 +1706,7 @@
       <c r="S33" s="16"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34" s="42"/>
+      <c r="A34" s="48"/>
       <c r="B34" s="10">
         <v>1.8160000000000001</v>
       </c>
@@ -1719,7 +1719,7 @@
       <c r="E34" s="10">
         <v>1.7969999999999999</v>
       </c>
-      <c r="F34" s="48"/>
+      <c r="F34" s="44"/>
       <c r="O34" s="16"/>
       <c r="P34" s="16"/>
       <c r="Q34" s="16"/>
@@ -1727,7 +1727,7 @@
       <c r="S34" s="16"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="40">
+      <c r="A35" s="46">
         <v>2.5</v>
       </c>
       <c r="B35" s="21">
@@ -1742,14 +1742,14 @@
       <c r="E35" s="22">
         <v>2.5</v>
       </c>
-      <c r="F35" s="46"/>
+      <c r="F35" s="42"/>
       <c r="O35" s="16"/>
       <c r="P35" s="16"/>
       <c r="Q35" s="16"/>
       <c r="R35" s="16"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="41"/>
+      <c r="A36" s="47"/>
       <c r="B36" s="21">
         <v>2.524</v>
       </c>
@@ -1762,14 +1762,14 @@
       <c r="E36" s="12">
         <v>2.5</v>
       </c>
-      <c r="F36" s="47"/>
+      <c r="F36" s="43"/>
       <c r="O36" s="16"/>
       <c r="P36" s="16"/>
       <c r="Q36" s="16"/>
       <c r="R36" s="16"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="41"/>
+      <c r="A37" s="47"/>
       <c r="B37" s="21">
         <v>2.4950000000000001</v>
       </c>
@@ -1782,14 +1782,14 @@
       <c r="E37" s="12">
         <v>2.5</v>
       </c>
-      <c r="F37" s="47"/>
+      <c r="F37" s="43"/>
       <c r="O37" s="16"/>
       <c r="P37" s="16"/>
       <c r="Q37" s="16"/>
       <c r="R37" s="16"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A38" s="41"/>
+      <c r="A38" s="47"/>
       <c r="B38" s="21">
         <v>2.524</v>
       </c>
@@ -1802,14 +1802,14 @@
       <c r="E38" s="12">
         <v>2.5</v>
       </c>
-      <c r="F38" s="47"/>
+      <c r="F38" s="43"/>
       <c r="O38" s="16"/>
       <c r="P38" s="16"/>
       <c r="Q38" s="16"/>
       <c r="R38" s="16"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="41"/>
+      <c r="A39" s="47"/>
       <c r="B39" s="21">
         <v>2.5099999999999998</v>
       </c>
@@ -1822,14 +1822,14 @@
       <c r="E39" s="12">
         <v>2.5</v>
       </c>
-      <c r="F39" s="47"/>
+      <c r="F39" s="43"/>
       <c r="O39" s="16"/>
       <c r="P39" s="16"/>
       <c r="Q39" s="16"/>
       <c r="R39" s="16"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" s="41"/>
+      <c r="A40" s="47"/>
       <c r="B40" s="21">
         <v>2.52</v>
       </c>
@@ -1842,14 +1842,14 @@
       <c r="E40" s="12">
         <v>2.5</v>
       </c>
-      <c r="F40" s="47"/>
+      <c r="F40" s="43"/>
       <c r="O40" s="16"/>
       <c r="P40" s="16"/>
       <c r="Q40" s="16"/>
       <c r="R40" s="16"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A41" s="41"/>
+      <c r="A41" s="47"/>
       <c r="B41" s="21">
         <v>2.5539999999999998</v>
       </c>
@@ -1862,14 +1862,14 @@
       <c r="E41" s="12">
         <v>2.5</v>
       </c>
-      <c r="F41" s="47"/>
+      <c r="F41" s="43"/>
       <c r="O41" s="16"/>
       <c r="P41" s="16"/>
       <c r="Q41" s="16"/>
       <c r="R41" s="16"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A42" s="41"/>
+      <c r="A42" s="47"/>
       <c r="B42" s="21">
         <v>2.524</v>
       </c>
@@ -1882,14 +1882,14 @@
       <c r="E42" s="12">
         <v>2.5</v>
       </c>
-      <c r="F42" s="47"/>
+      <c r="F42" s="43"/>
       <c r="O42" s="16"/>
       <c r="P42" s="16"/>
       <c r="Q42" s="16"/>
       <c r="R42" s="16"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A43" s="41"/>
+      <c r="A43" s="47"/>
       <c r="B43" s="21">
         <v>2.5339999999999998</v>
       </c>
@@ -1902,14 +1902,14 @@
       <c r="E43" s="12">
         <v>2.5</v>
       </c>
-      <c r="F43" s="47"/>
+      <c r="F43" s="43"/>
       <c r="O43" s="16"/>
       <c r="P43" s="16"/>
       <c r="Q43" s="16"/>
       <c r="R43" s="16"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A44" s="42"/>
+      <c r="A44" s="48"/>
       <c r="B44" s="13">
         <v>2.52</v>
       </c>
@@ -1922,7 +1922,7 @@
       <c r="E44" s="13">
         <v>2.5</v>
       </c>
-      <c r="F44" s="48"/>
+      <c r="F44" s="44"/>
       <c r="O44" s="16"/>
       <c r="P44" s="16"/>
       <c r="Q44" s="16"/>
@@ -1934,20 +1934,20 @@
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B49" s="49" t="s">
+      <c r="B49" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C49" s="49"/>
-      <c r="D49" s="49"/>
-      <c r="E49" s="49"/>
-      <c r="F49" s="49"/>
-      <c r="G49" s="49" t="s">
+      <c r="C49" s="45"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="45"/>
+      <c r="G49" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="H49" s="49"/>
-      <c r="I49" s="49"/>
-      <c r="J49" s="49"/>
-      <c r="K49" s="49"/>
+      <c r="H49" s="45"/>
+      <c r="I49" s="45"/>
+      <c r="J49" s="45"/>
+      <c r="K49" s="45"/>
     </row>
     <row r="50" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
@@ -2435,7 +2435,7 @@
       <c r="E62" s="2">
         <v>1.016</v>
       </c>
-      <c r="F62" s="46"/>
+      <c r="F62" s="42"/>
       <c r="G62" s="21">
         <f t="shared" si="1"/>
         <v>9.9999999999988987E-4</v>
@@ -2470,7 +2470,7 @@
       <c r="E63" s="2">
         <v>1.016</v>
       </c>
-      <c r="F63" s="47"/>
+      <c r="F63" s="43"/>
       <c r="G63" s="21">
         <f t="shared" si="1"/>
         <v>9.9999999999988987E-4</v>
@@ -2505,7 +2505,7 @@
       <c r="E64" s="2">
         <v>1.016</v>
       </c>
-      <c r="F64" s="47"/>
+      <c r="F64" s="43"/>
       <c r="G64" s="21">
         <f t="shared" si="1"/>
         <v>9.9999999999988987E-4</v>
@@ -2540,7 +2540,7 @@
       <c r="E65" s="2">
         <v>1.016</v>
       </c>
-      <c r="F65" s="47"/>
+      <c r="F65" s="43"/>
       <c r="G65" s="21">
         <f t="shared" si="1"/>
         <v>9.9999999999988987E-4</v>
@@ -2575,7 +2575,7 @@
       <c r="E66" s="2">
         <v>1.016</v>
       </c>
-      <c r="F66" s="47"/>
+      <c r="F66" s="43"/>
       <c r="G66" s="21">
         <f t="shared" si="1"/>
         <v>9.9999999999988987E-4</v>
@@ -2610,7 +2610,7 @@
       <c r="E67" s="2">
         <v>1.016</v>
       </c>
-      <c r="F67" s="47"/>
+      <c r="F67" s="43"/>
       <c r="G67" s="21">
         <f t="shared" si="1"/>
         <v>9.9999999999988987E-4</v>
@@ -2645,7 +2645,7 @@
       <c r="E68" s="2">
         <v>1.016</v>
       </c>
-      <c r="F68" s="47"/>
+      <c r="F68" s="43"/>
       <c r="G68" s="21">
         <f t="shared" si="1"/>
         <v>9.9999999999988987E-4</v>
@@ -2680,7 +2680,7 @@
       <c r="E69" s="2">
         <v>1.016</v>
       </c>
-      <c r="F69" s="47"/>
+      <c r="F69" s="43"/>
       <c r="G69" s="21">
         <f t="shared" si="1"/>
         <v>9.9999999999988987E-4</v>
@@ -2715,7 +2715,7 @@
       <c r="E70" s="2">
         <v>1.016</v>
       </c>
-      <c r="F70" s="47"/>
+      <c r="F70" s="43"/>
       <c r="G70" s="21">
         <f t="shared" si="1"/>
         <v>9.9999999999988987E-4</v>
@@ -2750,7 +2750,7 @@
       <c r="E71" s="2">
         <v>1.016</v>
       </c>
-      <c r="F71" s="48"/>
+      <c r="F71" s="44"/>
       <c r="G71" s="21">
         <f t="shared" si="1"/>
         <v>9.9999999999988987E-4</v>
@@ -2785,7 +2785,7 @@
       <c r="E72" s="11">
         <v>1.7969999999999999</v>
       </c>
-      <c r="F72" s="46"/>
+      <c r="F72" s="42"/>
       <c r="G72" s="21">
         <f t="shared" si="1"/>
         <v>1.6000000000000014E-2</v>
@@ -2820,7 +2820,7 @@
       <c r="E73" s="2">
         <v>1.7969999999999999</v>
       </c>
-      <c r="F73" s="47"/>
+      <c r="F73" s="43"/>
       <c r="G73" s="21">
         <f t="shared" si="1"/>
         <v>2.0999999999999908E-2</v>
@@ -2855,7 +2855,7 @@
       <c r="E74" s="2">
         <v>1.7969999999999999</v>
       </c>
-      <c r="F74" s="47"/>
+      <c r="F74" s="43"/>
       <c r="G74" s="21">
         <f t="shared" si="1"/>
         <v>1.2000000000000011E-2</v>
@@ -2890,7 +2890,7 @@
       <c r="E75" s="2">
         <v>1.7969999999999999</v>
       </c>
-      <c r="F75" s="47"/>
+      <c r="F75" s="43"/>
       <c r="G75" s="21">
         <f t="shared" si="1"/>
         <v>1.6000000000000014E-2</v>
@@ -2925,7 +2925,7 @@
       <c r="E76" s="2">
         <v>1.7969999999999999</v>
       </c>
-      <c r="F76" s="47"/>
+      <c r="F76" s="43"/>
       <c r="G76" s="21">
         <f t="shared" si="1"/>
         <v>1.2000000000000011E-2</v>
@@ -2960,7 +2960,7 @@
       <c r="E77" s="2">
         <v>1.7969999999999999</v>
       </c>
-      <c r="F77" s="47"/>
+      <c r="F77" s="43"/>
       <c r="G77" s="21">
         <f t="shared" si="1"/>
         <v>1.2000000000000011E-2</v>
@@ -2995,7 +2995,7 @@
       <c r="E78" s="2">
         <v>1.7969999999999999</v>
       </c>
-      <c r="F78" s="47"/>
+      <c r="F78" s="43"/>
       <c r="G78" s="21">
         <f t="shared" si="1"/>
         <v>1.6000000000000014E-2</v>
@@ -3030,7 +3030,7 @@
       <c r="E79" s="2">
         <v>1.7969999999999999</v>
       </c>
-      <c r="F79" s="47"/>
+      <c r="F79" s="43"/>
       <c r="G79" s="21">
         <f t="shared" si="1"/>
         <v>1.6000000000000014E-2</v>
@@ -3083,7 +3083,7 @@
       <c r="E80" s="2">
         <v>1.7969999999999999</v>
       </c>
-      <c r="F80" s="47"/>
+      <c r="F80" s="43"/>
       <c r="G80" s="21">
         <f t="shared" si="1"/>
         <v>1.2000000000000011E-2</v>
@@ -3136,7 +3136,7 @@
       <c r="E81" s="10">
         <v>1.7969999999999999</v>
       </c>
-      <c r="F81" s="48"/>
+      <c r="F81" s="44"/>
       <c r="G81" s="21">
         <f t="shared" si="1"/>
         <v>1.6000000000000014E-2</v>
@@ -3189,7 +3189,7 @@
       <c r="E82" s="22">
         <v>2.5</v>
       </c>
-      <c r="F82" s="46"/>
+      <c r="F82" s="42"/>
       <c r="G82" s="21">
         <f t="shared" si="1"/>
         <v>2.0000000000000018E-2</v>
@@ -3242,7 +3242,7 @@
       <c r="E83" s="12">
         <v>2.5</v>
       </c>
-      <c r="F83" s="47"/>
+      <c r="F83" s="43"/>
       <c r="G83" s="21">
         <f t="shared" si="1"/>
         <v>2.4000000000000021E-2</v>
@@ -3295,7 +3295,7 @@
       <c r="E84" s="12">
         <v>2.5</v>
       </c>
-      <c r="F84" s="47"/>
+      <c r="F84" s="43"/>
       <c r="G84" s="21">
         <f t="shared" si="1"/>
         <v>2.0000000000000018E-2</v>
@@ -3348,7 +3348,7 @@
       <c r="E85" s="12">
         <v>2.5</v>
       </c>
-      <c r="F85" s="47"/>
+      <c r="F85" s="43"/>
       <c r="G85" s="21">
         <f t="shared" si="1"/>
         <v>2.4000000000000021E-2</v>
@@ -3401,7 +3401,7 @@
       <c r="E86" s="12">
         <v>2.5</v>
       </c>
-      <c r="F86" s="47"/>
+      <c r="F86" s="43"/>
       <c r="G86" s="21">
         <f t="shared" si="1"/>
         <v>9.9999999999997868E-3</v>
@@ -3454,7 +3454,7 @@
       <c r="E87" s="12">
         <v>2.5</v>
       </c>
-      <c r="F87" s="47"/>
+      <c r="F87" s="43"/>
       <c r="G87" s="21">
         <f t="shared" si="1"/>
         <v>2.0000000000000018E-2</v>
@@ -3507,7 +3507,7 @@
       <c r="E88" s="12">
         <v>2.5</v>
       </c>
-      <c r="F88" s="47"/>
+      <c r="F88" s="43"/>
       <c r="G88" s="21">
         <f t="shared" si="1"/>
         <v>5.3999999999999826E-2</v>
@@ -3560,7 +3560,7 @@
       <c r="E89" s="12">
         <v>2.5</v>
       </c>
-      <c r="F89" s="47"/>
+      <c r="F89" s="43"/>
       <c r="G89" s="21">
         <f t="shared" si="1"/>
         <v>2.4000000000000021E-2</v>
@@ -3610,7 +3610,7 @@
       <c r="E90" s="12">
         <v>2.5</v>
       </c>
-      <c r="F90" s="47"/>
+      <c r="F90" s="43"/>
       <c r="G90" s="21">
         <f t="shared" si="1"/>
         <v>3.3999999999999808E-2</v>
@@ -3660,7 +3660,7 @@
       <c r="E91" s="13">
         <v>2.5</v>
       </c>
-      <c r="F91" s="48"/>
+      <c r="F91" s="44"/>
       <c r="G91" s="21">
         <f t="shared" si="1"/>
         <v>2.0000000000000018E-2</v>
@@ -5473,11 +5473,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="F82:F91"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="G49:K49"/>
-    <mergeCell ref="F62:F71"/>
-    <mergeCell ref="F72:F81"/>
     <mergeCell ref="A5:A14"/>
     <mergeCell ref="A15:A24"/>
     <mergeCell ref="A25:A34"/>
@@ -5485,6 +5480,11 @@
     <mergeCell ref="F15:F24"/>
     <mergeCell ref="F25:F34"/>
     <mergeCell ref="F35:F44"/>
+    <mergeCell ref="F82:F91"/>
+    <mergeCell ref="B49:F49"/>
+    <mergeCell ref="G49:K49"/>
+    <mergeCell ref="F62:F71"/>
+    <mergeCell ref="F72:F81"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5550,14 +5550,14 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50" t="s">
+      <c r="C5" s="52"/>
+      <c r="D5" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="50"/>
+      <c r="E5" s="52"/>
       <c r="G5" s="19" t="s">
         <v>25</v>
       </c>
@@ -11149,7 +11149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C20DF4A1-8070-4F58-A040-71BC06857F9D}">
   <dimension ref="A1:AK74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="D3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
@@ -11175,10 +11175,10 @@
         <v>17</v>
       </c>
       <c r="B1" s="7"/>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="50"/>
+      <c r="D1" s="52"/>
       <c r="K1" s="33" t="s">
         <v>46</v>
       </c>
@@ -11217,13 +11217,13 @@
       <c r="L2" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="O2" s="51" t="s">
+      <c r="O2" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
@@ -11372,7 +11372,7 @@
         <f>A62-A50</f>
         <v>21400</v>
       </c>
-      <c r="T5" s="52">
+      <c r="T5" s="40">
         <f>AVERAGE(O5:S5)</f>
         <v>21157.599999999999</v>
       </c>
@@ -11388,13 +11388,13 @@
         <f>V5*U5/SQRT(5)</f>
         <v>182.10093666651801</v>
       </c>
-      <c r="AB5" s="51" t="s">
+      <c r="AB5" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="AC5" s="51"/>
-      <c r="AD5" s="51"/>
-      <c r="AE5" s="51"/>
-      <c r="AF5" s="51"/>
+      <c r="AC5" s="53"/>
+      <c r="AD5" s="53"/>
+      <c r="AE5" s="53"/>
+      <c r="AF5" s="53"/>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -11448,7 +11448,7 @@
         <f>C62-C50</f>
         <v>21304</v>
       </c>
-      <c r="T6" s="52">
+      <c r="T6" s="40">
         <f>AVERAGE(O6:S6)</f>
         <v>21110.400000000001</v>
       </c>
@@ -11526,23 +11526,23 @@
         <v>10</v>
       </c>
       <c r="AB7" s="21">
-        <f>1/O5*10^6</f>
+        <f t="shared" ref="AB7:AF8" si="4">1/O5*10^6</f>
         <v>47.61904761904762</v>
       </c>
       <c r="AC7" s="21">
-        <f>1/P5*10^6</f>
+        <f t="shared" si="4"/>
         <v>47.321597577134206</v>
       </c>
       <c r="AD7" s="21">
-        <f>1/Q5*10^6</f>
+        <f t="shared" si="4"/>
         <v>47.321597577134206</v>
       </c>
       <c r="AE7" s="21">
-        <f>1/R5*10^6</f>
+        <f t="shared" si="4"/>
         <v>47.339519030486649</v>
       </c>
       <c r="AF7" s="21">
-        <f>1/S5*10^6</f>
+        <f t="shared" si="4"/>
         <v>46.728971962616818</v>
       </c>
       <c r="AG7">
@@ -11601,23 +11601,23 @@
         <v>5</v>
       </c>
       <c r="AB8" s="21">
-        <f>1/O6*10^6</f>
+        <f t="shared" si="4"/>
         <v>47.819433817903594</v>
       </c>
       <c r="AC8" s="21">
-        <f>1/P6*10^6</f>
+        <f t="shared" si="4"/>
         <v>47.384382107657316</v>
       </c>
       <c r="AD8" s="21">
-        <f>1/Q6*10^6</f>
+        <f t="shared" si="4"/>
         <v>47.312641937925811</v>
       </c>
       <c r="AE8" s="21">
-        <f>1/R6*10^6</f>
+        <f t="shared" si="4"/>
         <v>47.402351156617364</v>
       </c>
       <c r="AF8" s="21">
-        <f>1/S6*10^6</f>
+        <f t="shared" si="4"/>
         <v>46.939541870071345</v>
       </c>
       <c r="AG8">
@@ -11727,13 +11727,13 @@
         <f>W5/(T5)^2*10^6</f>
         <v>0.40679853031830099</v>
       </c>
-      <c r="AB10" s="51" t="s">
+      <c r="AB10" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="AC10" s="51"/>
-      <c r="AD10" s="51"/>
-      <c r="AE10" s="51"/>
-      <c r="AF10" s="51"/>
+      <c r="AC10" s="53"/>
+      <c r="AD10" s="53"/>
+      <c r="AE10" s="53"/>
+      <c r="AF10" s="53"/>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -11871,7 +11871,7 @@
         <v>2.7764451051977934</v>
       </c>
       <c r="AJ12" s="25">
-        <f t="shared" ref="AJ12:AJ13" si="4">AI12*AH12/SQRT(5)</f>
+        <f t="shared" ref="AJ12:AJ13" si="5">AI12*AH12/SQRT(5)</f>
         <v>2.0098087593650941E-2</v>
       </c>
       <c r="AK12" s="25">
@@ -11908,13 +11908,13 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O13" s="51" t="s">
+      <c r="O13" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="P13" s="51"/>
-      <c r="Q13" s="51"/>
-      <c r="R13" s="51"/>
-      <c r="S13" s="51"/>
+      <c r="P13" s="53"/>
+      <c r="Q13" s="53"/>
+      <c r="R13" s="53"/>
+      <c r="S13" s="53"/>
       <c r="AA13">
         <v>5</v>
       </c>
@@ -11951,7 +11951,7 @@
         <v>2.7764451051977934</v>
       </c>
       <c r="AJ13" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.1373217966375407E-2</v>
       </c>
       <c r="AK13" s="25">
@@ -12155,19 +12155,19 @@
         <v>0.55100000000000005</v>
       </c>
       <c r="T16">
-        <f t="shared" ref="T16:T18" si="5">AVERAGE(O16:S16)</f>
+        <f t="shared" ref="T16:T18" si="6">AVERAGE(O16:S16)</f>
         <v>0.54200000000000004</v>
       </c>
       <c r="U16" s="31">
-        <f t="shared" ref="U16:U18" si="6">_xlfn.STDEV.S(O16:S16)</f>
+        <f t="shared" ref="U16:U18" si="7">_xlfn.STDEV.S(O16:S16)</f>
         <v>8.3066238629180816E-3</v>
       </c>
       <c r="V16" s="25">
-        <f t="shared" ref="V16:V18" si="7">-_xlfn.T.INV(0.025, 4)</f>
+        <f t="shared" ref="V16:V18" si="8">-_xlfn.T.INV(0.025, 4)</f>
         <v>2.7764451051977934</v>
       </c>
       <c r="W16" s="39">
-        <f t="shared" ref="W16:W18" si="8">V16*U16/SQRT(5)</f>
+        <f t="shared" ref="W16:W18" si="9">V16*U16/SQRT(5)</f>
         <v>1.0314035797205662E-2</v>
       </c>
       <c r="X16" s="39">
@@ -12175,7 +12175,7 @@
         <v>5.1562499999999997E-2</v>
       </c>
       <c r="Y16" s="25">
-        <f t="shared" ref="Y16:Y18" si="9">SQRT(W16^2+X16^2)</f>
+        <f t="shared" ref="Y16:Y18" si="10">SQRT(W16^2+X16^2)</f>
         <v>5.2583939950103013E-2</v>
       </c>
       <c r="AG16" t="s">
@@ -12238,19 +12238,19 @@
         <v>1.76</v>
       </c>
       <c r="T17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.7609999999999999</v>
       </c>
       <c r="U17" s="31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.2736184954956696E-3</v>
       </c>
       <c r="V17" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.7764451051977934</v>
       </c>
       <c r="W17" s="39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.1514718218933529E-2</v>
       </c>
       <c r="X17" s="39">
@@ -12258,7 +12258,7 @@
         <v>1.6999999999999904E-2</v>
       </c>
       <c r="Y17" s="25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.0532626126763143E-2</v>
       </c>
       <c r="AG17" t="s">
@@ -12327,19 +12327,19 @@
         <v>1.766</v>
       </c>
       <c r="T18" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.7614000000000001</v>
       </c>
       <c r="U18" s="31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.0922453936730473E-2</v>
       </c>
       <c r="V18" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2.7764451051977934</v>
       </c>
       <c r="W18" s="39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.3562017825277202E-2</v>
       </c>
       <c r="X18" s="39">
@@ -12347,7 +12347,7 @@
         <v>5.1562499999999997E-2</v>
       </c>
       <c r="Y18" s="25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.3316223926147814E-2</v>
       </c>
       <c r="AF18" t="s">
@@ -12451,28 +12451,28 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O20" s="53" t="str">
-        <f t="shared" ref="O20:T24" si="10">T14</f>
+      <c r="O20" s="41" t="str">
+        <f t="shared" ref="O20:T20" si="11">T14</f>
         <v>Nominal Value</v>
       </c>
-      <c r="P20" s="53" t="str">
-        <f t="shared" si="10"/>
+      <c r="P20" s="41" t="str">
+        <f t="shared" si="11"/>
         <v>Stdev</v>
       </c>
-      <c r="Q20" s="53" t="str">
-        <f t="shared" si="10"/>
+      <c r="Q20" s="41" t="str">
+        <f t="shared" si="11"/>
         <v>T INV</v>
       </c>
-      <c r="R20" s="53" t="str">
-        <f t="shared" si="10"/>
+      <c r="R20" s="41" t="str">
+        <f t="shared" si="11"/>
         <v>P_x</v>
       </c>
-      <c r="S20" s="53" t="str">
-        <f t="shared" si="10"/>
+      <c r="S20" s="41" t="str">
+        <f t="shared" si="11"/>
         <v>B_x</v>
       </c>
-      <c r="T20" s="53" t="str">
-        <f t="shared" si="10"/>
+      <c r="T20" s="41" t="str">
+        <f t="shared" si="11"/>
         <v>U_x</v>
       </c>
       <c r="AA20" s="33" t="s">
@@ -12518,27 +12518,27 @@
         <v>84</v>
       </c>
       <c r="O21">
-        <f t="shared" ref="O21:T24" si="11">T15</f>
+        <f t="shared" ref="O21:T24" si="12">T15</f>
         <v>0.54400000000000004</v>
       </c>
       <c r="P21" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.1113055385446446E-2</v>
       </c>
       <c r="Q21" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.7764451051977934</v>
       </c>
       <c r="R21" s="39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.3798680782153308E-2</v>
       </c>
       <c r="S21" s="39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.6999999999999904E-2</v>
       </c>
       <c r="T21" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.1895286966097608E-2</v>
       </c>
       <c r="Z21" s="33" t="s">
@@ -12590,27 +12590,27 @@
         <v>85</v>
       </c>
       <c r="O22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.54200000000000004</v>
       </c>
       <c r="P22" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>8.3066238629180816E-3</v>
       </c>
       <c r="Q22" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.7764451051977934</v>
       </c>
       <c r="R22" s="39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.0314035797205662E-2</v>
       </c>
       <c r="S22" s="39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5.1562499999999997E-2</v>
       </c>
       <c r="T22" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5.2583939950103013E-2</v>
       </c>
       <c r="Z22" s="33" t="s">
@@ -12662,27 +12662,27 @@
         <v>86</v>
       </c>
       <c r="O23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.7609999999999999</v>
       </c>
       <c r="P23" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>9.2736184954956696E-3</v>
       </c>
       <c r="Q23" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.7764451051977934</v>
       </c>
       <c r="R23" s="39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.1514718218933529E-2</v>
       </c>
       <c r="S23" s="39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.6999999999999904E-2</v>
       </c>
       <c r="T23" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.0532626126763143E-2</v>
       </c>
       <c r="Z23" t="s">
@@ -12731,27 +12731,27 @@
         <v>87</v>
       </c>
       <c r="O24" s="21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.7614000000000001</v>
       </c>
       <c r="P24" s="31">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.0922453936730473E-2</v>
       </c>
       <c r="Q24" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2.7764451051977934</v>
       </c>
       <c r="R24" s="39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.3562017825277202E-2</v>
       </c>
       <c r="S24" s="39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5.1562499999999997E-2</v>
       </c>
       <c r="T24" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5.3316223926147814E-2</v>
       </c>
     </row>
@@ -12844,7 +12844,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O27" s="53" t="s">
+      <c r="O27" s="41" t="s">
         <v>89</v>
       </c>
       <c r="P27" t="s">
@@ -13585,11 +13585,11 @@
         <v>1</v>
       </c>
       <c r="G51" t="b">
-        <f t="shared" ref="G51:G73" si="12">B51&gt;1.7</f>
+        <f t="shared" ref="G51:G73" si="13">B51&gt;1.7</f>
         <v>0</v>
       </c>
       <c r="H51" t="b">
-        <f t="shared" ref="H51:H73" si="13">D51&gt;1.7</f>
+        <f t="shared" ref="H51:H73" si="14">D51&gt;1.7</f>
         <v>0</v>
       </c>
     </row>
@@ -13615,11 +13615,11 @@
         <v>0</v>
       </c>
       <c r="G52" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H52" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -13645,11 +13645,11 @@
         <v>0</v>
       </c>
       <c r="G53" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H53" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -13675,11 +13675,11 @@
         <v>0</v>
       </c>
       <c r="G54" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H54" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -13705,11 +13705,11 @@
         <v>0</v>
       </c>
       <c r="G55" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H55" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -13735,11 +13735,11 @@
         <v>0</v>
       </c>
       <c r="G56" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="H56" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
     </row>
@@ -13765,11 +13765,11 @@
         <v>0</v>
       </c>
       <c r="G57" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="H57" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
     </row>
@@ -13795,11 +13795,11 @@
         <v>0</v>
       </c>
       <c r="G58" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H58" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -13825,11 +13825,11 @@
         <v>0</v>
       </c>
       <c r="G59" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H59" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -13855,11 +13855,11 @@
         <v>0</v>
       </c>
       <c r="G60" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H60" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -13885,11 +13885,11 @@
         <v>0</v>
       </c>
       <c r="G61" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H61" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -13915,11 +13915,11 @@
         <v>1</v>
       </c>
       <c r="G62" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H62" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -13945,11 +13945,11 @@
         <v>0</v>
       </c>
       <c r="G63" s="38" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H63" s="38" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -13975,11 +13975,11 @@
         <v>0</v>
       </c>
       <c r="G64" s="38" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H64" s="38" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -14005,11 +14005,11 @@
         <v>0</v>
       </c>
       <c r="G65" s="38" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H65" s="38" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -14035,11 +14035,11 @@
         <v>0</v>
       </c>
       <c r="G66" s="38" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H66" s="38" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -14065,11 +14065,11 @@
         <v>0</v>
       </c>
       <c r="G67" s="38" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H67" s="38" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
     </row>
@@ -14087,19 +14087,19 @@
         <v>1.76</v>
       </c>
       <c r="E68" s="38" t="b">
-        <f t="shared" ref="E68:E74" si="14">B68&lt;0.6</f>
+        <f t="shared" ref="E68:E74" si="15">B68&lt;0.6</f>
         <v>0</v>
       </c>
       <c r="F68" s="38" t="b">
-        <f t="shared" ref="F68:F73" si="15">D68&lt;0.6</f>
+        <f t="shared" ref="F68:F73" si="16">D68&lt;0.6</f>
         <v>0</v>
       </c>
       <c r="G68" s="38" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="H68" s="38" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
     </row>
@@ -14117,19 +14117,19 @@
         <v>1.6080000000000001</v>
       </c>
       <c r="E69" s="38" t="b">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="F69" s="38" t="b">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="G69" s="38" t="b">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="H69" s="38" t="b">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="F69" s="38" t="b">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="G69" s="38" t="b">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="H69" s="38" t="b">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -14147,19 +14147,19 @@
         <v>1.3540000000000001</v>
       </c>
       <c r="E70" s="38" t="b">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="F70" s="38" t="b">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="G70" s="38" t="b">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="H70" s="38" t="b">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="F70" s="38" t="b">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="G70" s="38" t="b">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="H70" s="38" t="b">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -14177,19 +14177,19 @@
         <v>1.0629999999999999</v>
       </c>
       <c r="E71" s="38" t="b">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="F71" s="38" t="b">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="G71" s="38" t="b">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="H71" s="38" t="b">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="F71" s="38" t="b">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="G71" s="38" t="b">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="H71" s="38" t="b">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -14207,19 +14207,19 @@
         <v>0.78300000000000003</v>
       </c>
       <c r="E72" s="38" t="b">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="F72" s="38" t="b">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="G72" s="38" t="b">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="H72" s="38" t="b">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="F72" s="38" t="b">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="G72" s="38" t="b">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="H72" s="38" t="b">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
@@ -14237,19 +14237,19 @@
         <v>0.55800000000000005</v>
       </c>
       <c r="E73" s="38" t="b">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="F73" s="38" t="b">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
+      <c r="F73" s="38" t="b">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
       <c r="G73" s="38" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H73" s="38" t="b">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -14263,7 +14263,7 @@
       <c r="C74" s="38"/>
       <c r="D74" s="38"/>
       <c r="E74" s="38" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="F74" s="38"/>

</xml_diff>